<commit_message>
Changed locations to Proper Casing
The locations were all in capitals. I converted the data to be proper
casing so that it stopped yelling
</commit_message>
<xml_diff>
--- a/misc files/ACT - BBQ locations.xlsx
+++ b/misc files/ACT - BBQ locations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23070" windowHeight="10320" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23070" windowHeight="10320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1182" uniqueCount="275">
   <si>
     <t>IIT_NE_ID</t>
   </si>
@@ -842,6 +842,9 @@
   </si>
   <si>
     <t>C# ViewModel</t>
+  </si>
+  <si>
+    <t>proper casing</t>
   </si>
 </sst>
 </file>
@@ -1214,10 +1217,10 @@
   <sheetPr>
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:U102"/>
+  <dimension ref="A1:V102"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99:IV99"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1244,7 +1247,7 @@
     <col min="20" max="256" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1308,8 +1311,11 @@
       <c r="U1" s="8" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V1" s="8" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>4325150</v>
       </c>
@@ -1361,8 +1367,12 @@
       <c r="U2">
         <v>149.08430638361111</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V2" t="str">
+        <f>PROPER(N2)</f>
+        <v>Point Hut District Park</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>4223956</v>
       </c>
@@ -1420,8 +1430,12 @@
       <c r="U3">
         <v>149.15100653166667</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V3" t="str">
+        <f t="shared" ref="V3:V66" si="0">PROPER(N3)</f>
+        <v>Rememberance Park</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>4223982</v>
       </c>
@@ -1477,8 +1491,12 @@
       <c r="U4">
         <v>149.15126871777778</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V4" t="str">
+        <f t="shared" si="0"/>
+        <v>Rememberance Park</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2524152</v>
       </c>
@@ -1540,8 +1558,12 @@
       <c r="U5">
         <v>149.09026374277778</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V5" t="str">
+        <f t="shared" si="0"/>
+        <v>Edison District Park</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2524153</v>
       </c>
@@ -1601,8 +1623,12 @@
       <c r="U6">
         <v>149.0900415952778</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V6" t="str">
+        <f t="shared" si="0"/>
+        <v>Edison District Park</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>2524154</v>
       </c>
@@ -1664,8 +1690,12 @@
       <c r="U7">
         <v>149.08315695666667</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V7" t="str">
+        <f t="shared" si="0"/>
+        <v>Phillip Town Centre</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>2524155</v>
       </c>
@@ -1727,8 +1757,12 @@
       <c r="U8">
         <v>149.08691370944445</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V8" t="str">
+        <f t="shared" si="0"/>
+        <v>Phillip Town Centre</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>2524156</v>
       </c>
@@ -1790,8 +1824,12 @@
       <c r="U9">
         <v>149.08897375000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V9" t="str">
+        <f t="shared" si="0"/>
+        <v>Groom Street - Pedestrian Parkland</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2524157</v>
       </c>
@@ -1853,8 +1891,12 @@
       <c r="U10">
         <v>149.05728793500001</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V10" t="str">
+        <f t="shared" si="0"/>
+        <v>Araluen Street - Neighbourhood Park</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>2524158</v>
       </c>
@@ -1916,8 +1958,12 @@
       <c r="U11">
         <v>149.13324905416667</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V11" t="str">
+        <f t="shared" si="0"/>
+        <v>Lowanna Street - Neighbourhood Park</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>2524159</v>
       </c>
@@ -1973,8 +2019,12 @@
       <c r="U12">
         <v>149.13397897888888</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V12" t="str">
+        <f t="shared" si="0"/>
+        <v>Lowanna Street - Neighbourhood Park</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>2524163</v>
       </c>
@@ -2036,8 +2086,12 @@
       <c r="U13">
         <v>149.12844226750002</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V13" t="str">
+        <f t="shared" si="0"/>
+        <v>Haig Park</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>2524164</v>
       </c>
@@ -2099,8 +2153,12 @@
       <c r="U14">
         <v>149.12652939861113</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V14" t="str">
+        <f t="shared" si="0"/>
+        <v>Haig Park</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>2524165</v>
       </c>
@@ -2162,8 +2220,12 @@
       <c r="U15">
         <v>149.14236726472222</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V15" t="str">
+        <f t="shared" si="0"/>
+        <v>Corroboree Park</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>2524166</v>
       </c>
@@ -2225,8 +2287,12 @@
       <c r="U16">
         <v>149.13638735277777</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V16" t="str">
+        <f t="shared" si="0"/>
+        <v>Glebe Park</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>2524167</v>
       </c>
@@ -2288,8 +2354,12 @@
       <c r="U17">
         <v>149.13664595027777</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V17" t="str">
+        <f t="shared" si="0"/>
+        <v>Glebe Park</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>2524168</v>
       </c>
@@ -2351,8 +2421,12 @@
       <c r="U18">
         <v>149.13634045222221</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V18" t="str">
+        <f t="shared" si="0"/>
+        <v>Glebe Park</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>2524171</v>
       </c>
@@ -2414,8 +2488,12 @@
       <c r="U19">
         <v>149.16736595166665</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V19" t="str">
+        <f t="shared" si="0"/>
+        <v>Molonglo Reach District Park</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>2524172</v>
       </c>
@@ -2477,8 +2555,12 @@
       <c r="U20">
         <v>149.10143369333332</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V20" t="str">
+        <f t="shared" si="0"/>
+        <v>Black Mountain Peninsula District Park</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>2524173</v>
       </c>
@@ -2540,8 +2622,12 @@
       <c r="U21">
         <v>149.09958337638889</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V21" t="str">
+        <f t="shared" si="0"/>
+        <v>Black Mountain Peninsula District Park</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>2524174</v>
       </c>
@@ -2603,8 +2689,12 @@
       <c r="U22">
         <v>149.1001386675</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V22" t="str">
+        <f t="shared" si="0"/>
+        <v>Black Mountain Peninsula District Park</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>2524175</v>
       </c>
@@ -2666,8 +2756,12 @@
       <c r="U23">
         <v>149.10097284833333</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V23" t="str">
+        <f t="shared" si="0"/>
+        <v>Black Mountain Peninsula District Park</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>2524176</v>
       </c>
@@ -2729,8 +2823,12 @@
       <c r="U24">
         <v>149.12472294388888</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V24" t="str">
+        <f t="shared" si="0"/>
+        <v>Acton Park District Park</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>2524177</v>
       </c>
@@ -2792,8 +2890,12 @@
       <c r="U25">
         <v>149.12439368611112</v>
       </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V25" t="str">
+        <f t="shared" si="0"/>
+        <v>Acton Park District Park</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>2524178</v>
       </c>
@@ -2855,8 +2957,12 @@
       <c r="U26">
         <v>149.07421343305555</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V26" t="str">
+        <f t="shared" si="0"/>
+        <v>Ginninderra Peninsula District Park</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>2524179</v>
       </c>
@@ -2918,8 +3024,12 @@
       <c r="U27">
         <v>149.07401866972222</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V27" t="str">
+        <f t="shared" si="0"/>
+        <v>Diddams Close Pedestrian Parkland</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>2524180</v>
       </c>
@@ -2981,8 +3091,12 @@
       <c r="U28">
         <v>149.0627282677778</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V28" t="str">
+        <f t="shared" si="0"/>
+        <v>Joynton Smith Drive Pedestrian Parkland</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>2524181</v>
       </c>
@@ -3046,8 +3160,12 @@
       <c r="U29">
         <v>149.06344848222224</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V29" t="str">
+        <f t="shared" si="0"/>
+        <v>Lake Ginninderra Western Foreshores</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>2524182</v>
       </c>
@@ -3109,8 +3227,12 @@
       <c r="U30">
         <v>149.06337945222222</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V30" t="str">
+        <f t="shared" si="0"/>
+        <v>Lake Ginninderra Western Foreshores</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>2524183</v>
       </c>
@@ -3174,8 +3296,12 @@
       <c r="U31">
         <v>149.06318664083335</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V31" t="str">
+        <f t="shared" si="0"/>
+        <v>Lake Ginninderra Western Foreshores</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>2524184</v>
       </c>
@@ -3237,8 +3363,12 @@
       <c r="U32">
         <v>149.0632299225</v>
       </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V32" t="str">
+        <f t="shared" si="0"/>
+        <v>Lake Ginninderra Western Foreshores</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>2524185</v>
       </c>
@@ -3302,8 +3432,12 @@
       <c r="U33">
         <v>149.06282296194445</v>
       </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V33" t="str">
+        <f t="shared" si="0"/>
+        <v>Lake Ginninderra Western Foreshores</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>2524186</v>
       </c>
@@ -3359,8 +3493,12 @@
       <c r="U34">
         <v>149.06028199944444</v>
       </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V34" t="str">
+        <f t="shared" si="0"/>
+        <v>Totterdell Street Pedestrian Parkland</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>2524187</v>
       </c>
@@ -3422,8 +3560,12 @@
       <c r="U35">
         <v>149.06960032500001</v>
       </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V35" t="str">
+        <f t="shared" si="0"/>
+        <v>Ginninderra Peninsula District Park</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>2524188</v>
       </c>
@@ -3485,8 +3627,12 @@
       <c r="U36">
         <v>149.06942067444444</v>
       </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V36" t="str">
+        <f t="shared" si="0"/>
+        <v>Ginninderra Peninsula District Park</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>2524189</v>
       </c>
@@ -3548,8 +3694,12 @@
       <c r="U37">
         <v>149.07337771444443</v>
       </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V37" t="str">
+        <f t="shared" si="0"/>
+        <v>John Knight Memorial Park</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>2524190</v>
       </c>
@@ -3611,8 +3761,12 @@
       <c r="U38">
         <v>149.07336354888889</v>
       </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V38" t="str">
+        <f t="shared" si="0"/>
+        <v>John Knight Memorial Park</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>2524191</v>
       </c>
@@ -3668,8 +3822,12 @@
       <c r="U39">
         <v>149.06710429638889</v>
       </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V39" t="str">
+        <f t="shared" si="0"/>
+        <v>Carlile Street Pedestrian Parkland</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>2524192</v>
       </c>
@@ -3725,8 +3883,12 @@
       <c r="U40">
         <v>149.05692773666667</v>
       </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V40" t="str">
+        <f t="shared" si="0"/>
+        <v>Tattersall Crescent Neighbourhood Park</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>2524193</v>
       </c>
@@ -3782,8 +3944,12 @@
       <c r="U41">
         <v>149.06970083277778</v>
       </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V41" t="str">
+        <f t="shared" si="0"/>
+        <v>Hall Park</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>2524194</v>
       </c>
@@ -3839,8 +4005,12 @@
       <c r="U42">
         <v>149.06978448916666</v>
       </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V42" t="str">
+        <f t="shared" si="0"/>
+        <v>Hall Park</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>2524195</v>
       </c>
@@ -3904,8 +4074,12 @@
       <c r="U43">
         <v>149.03109260166667</v>
       </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V43" t="str">
+        <f t="shared" si="0"/>
+        <v>Umbagong District Park</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>2524196</v>
       </c>
@@ -3969,8 +4143,12 @@
       <c r="U44">
         <v>149.0288525777778</v>
       </c>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V44" t="str">
+        <f t="shared" si="0"/>
+        <v>Umbagong District Park</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>2524197</v>
       </c>
@@ -4034,8 +4212,12 @@
       <c r="U45">
         <v>149.02898493666669</v>
       </c>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V45" t="str">
+        <f t="shared" si="0"/>
+        <v>Umbagong District Park</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>2524198</v>
       </c>
@@ -4099,8 +4281,12 @@
       <c r="U46">
         <v>149.01409828777778</v>
       </c>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V46" t="str">
+        <f t="shared" si="0"/>
+        <v>Marks Place Pedestrian Parkland</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>2524199</v>
       </c>
@@ -4164,8 +4350,12 @@
       <c r="U47">
         <v>149.01479495555554</v>
       </c>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V47" t="str">
+        <f t="shared" si="0"/>
+        <v>Harper Street Pedestrian Parkland</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>2524200</v>
       </c>
@@ -4229,8 +4419,12 @@
       <c r="U48">
         <v>149.08574079027778</v>
       </c>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V48" t="str">
+        <f t="shared" si="0"/>
+        <v>Palmerville Heritage Park</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>2524201</v>
       </c>
@@ -4294,8 +4488,12 @@
       <c r="U49">
         <v>149.08555615916669</v>
       </c>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V49" t="str">
+        <f t="shared" si="0"/>
+        <v>Palmerville Heritage Park</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>2524204</v>
       </c>
@@ -4353,8 +4551,12 @@
       <c r="U50">
         <v>149.13063986083333</v>
       </c>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V50" t="str">
+        <f t="shared" si="0"/>
+        <v>Yerrabi District Park</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>2524205</v>
       </c>
@@ -4412,8 +4614,12 @@
       <c r="U51">
         <v>149.13087482500001</v>
       </c>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V51" t="str">
+        <f t="shared" si="0"/>
+        <v>Yerrabi District Park</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>2524206</v>
       </c>
@@ -4471,8 +4677,12 @@
       <c r="U52">
         <v>149.1308299625</v>
       </c>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V52" t="str">
+        <f t="shared" si="0"/>
+        <v>Yerrabi District Park</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>2524207</v>
       </c>
@@ -4530,8 +4740,12 @@
       <c r="U53">
         <v>149.1306033686111</v>
       </c>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V53" t="str">
+        <f t="shared" si="0"/>
+        <v>Yerrabi District Park</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>2524208</v>
       </c>
@@ -4587,8 +4801,12 @@
       <c r="U54">
         <v>149.14218595333332</v>
       </c>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V54" t="str">
+        <f t="shared" si="0"/>
+        <v>Baillieu Lane Pedestrian Parkland</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>2524209</v>
       </c>
@@ -4644,8 +4862,12 @@
       <c r="U55">
         <v>149.08394238972224</v>
       </c>
-    </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V55" t="str">
+        <f t="shared" si="0"/>
+        <v>Griffin Place - Pedestrian Parkland</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>2524210</v>
       </c>
@@ -4701,8 +4923,12 @@
       <c r="U56">
         <v>149.07878835194444</v>
       </c>
-    </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V56" t="str">
+        <f t="shared" si="0"/>
+        <v>Newman-Morris Circuit - Neighbourhood Park</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>2524211</v>
       </c>
@@ -4764,8 +4990,12 @@
       <c r="U57">
         <v>149.06053032055556</v>
       </c>
-    </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V57" t="str">
+        <f t="shared" si="0"/>
+        <v>Kambah District Park</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>2524212</v>
       </c>
@@ -4827,8 +5057,12 @@
       <c r="U58">
         <v>149.06043036111112</v>
       </c>
-    </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V58" t="str">
+        <f t="shared" si="0"/>
+        <v>Kambah District Park</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>2524213</v>
       </c>
@@ -4890,8 +5124,12 @@
       <c r="U59">
         <v>149.06214088166666</v>
       </c>
-    </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V59" t="str">
+        <f t="shared" si="0"/>
+        <v>Kambah District Park</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>2524214</v>
       </c>
@@ -4953,8 +5191,12 @@
       <c r="U60">
         <v>149.06208656333334</v>
       </c>
-    </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V60" t="str">
+        <f t="shared" si="0"/>
+        <v>Kambah District Park</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>2524215</v>
       </c>
@@ -5016,8 +5258,12 @@
       <c r="U61">
         <v>149.06202186416667</v>
       </c>
-    </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V61" t="str">
+        <f t="shared" si="0"/>
+        <v>Kambah District Park</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>2524216</v>
       </c>
@@ -5079,8 +5325,12 @@
       <c r="U62">
         <v>149.06473373416668</v>
       </c>
-    </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V62" t="str">
+        <f t="shared" si="0"/>
+        <v>Tuggeranong Town Park</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>2524217</v>
       </c>
@@ -5136,8 +5386,12 @@
       <c r="U63">
         <v>149.08469713972224</v>
       </c>
-    </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V63" t="str">
+        <f t="shared" si="0"/>
+        <v>Point Hut District Park</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>2524218</v>
       </c>
@@ -5193,8 +5447,12 @@
       <c r="U64">
         <v>149.17666069694442</v>
       </c>
-    </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V64" t="str">
+        <f t="shared" si="0"/>
+        <v>Maryborough Street - Pedestrian Parkland</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>2524219</v>
       </c>
@@ -5250,8 +5508,12 @@
       <c r="U65">
         <v>149.17657863083332</v>
       </c>
-    </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V65" t="str">
+        <f t="shared" si="0"/>
+        <v>Maryborough Street - Pedestrian Parkland</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>2524220</v>
       </c>
@@ -5315,8 +5577,12 @@
       <c r="U66">
         <v>149.11207327388888</v>
       </c>
-    </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V66" t="str">
+        <f t="shared" si="0"/>
+        <v>Bedford Street - Neighbourhood Park</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>2524221</v>
       </c>
@@ -5378,8 +5644,12 @@
       <c r="U67">
         <v>149.1372983536111</v>
       </c>
-    </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V67" t="str">
+        <f t="shared" ref="V67:V102" si="1">PROPER(N67)</f>
+        <v>Telopea Park</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>2524222</v>
       </c>
@@ -5441,8 +5711,12 @@
       <c r="U68">
         <v>149.13719974361109</v>
       </c>
-    </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V68" t="str">
+        <f t="shared" si="1"/>
+        <v>Telopea Park</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>2524224</v>
       </c>
@@ -5504,8 +5778,12 @@
       <c r="U69">
         <v>149.1377928025</v>
       </c>
-    </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V69" t="str">
+        <f t="shared" si="1"/>
+        <v>Telopea Park</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>2524225</v>
       </c>
@@ -5567,8 +5845,12 @@
       <c r="U70">
         <v>149.14014497777777</v>
       </c>
-    </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V70" t="str">
+        <f t="shared" si="1"/>
+        <v>Telopea Park</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>5823000</v>
       </c>
@@ -5622,8 +5904,12 @@
       <c r="U71">
         <v>149.13634045222221</v>
       </c>
-    </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V71" t="str">
+        <f t="shared" si="1"/>
+        <v>Telopea Park</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>2524226</v>
       </c>
@@ -5685,8 +5971,12 @@
       <c r="U72">
         <v>149.10926652277777</v>
       </c>
-    </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V72" t="str">
+        <f t="shared" si="1"/>
+        <v>Alexandrina Drive - Pedestrian Parkland</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>2524227</v>
       </c>
@@ -5748,8 +6038,12 @@
       <c r="U73">
         <v>149.11060368638888</v>
       </c>
-    </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V73" t="str">
+        <f t="shared" si="1"/>
+        <v>Alexandrina Drive - Pedestrian Parkland</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>2524228</v>
       </c>
@@ -5811,8 +6105,12 @@
       <c r="U74">
         <v>149.12108222472224</v>
       </c>
-    </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V74" t="str">
+        <f t="shared" si="1"/>
+        <v>Lennox Gardens</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>2524229</v>
       </c>
@@ -5874,8 +6172,12 @@
       <c r="U75">
         <v>149.12145216499999</v>
       </c>
-    </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V75" t="str">
+        <f t="shared" si="1"/>
+        <v>Lennox Gardens</v>
+      </c>
+    </row>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>2524230</v>
       </c>
@@ -5937,8 +6239,12 @@
       <c r="U76">
         <v>149.1218063588889</v>
       </c>
-    </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V76" t="str">
+        <f t="shared" si="1"/>
+        <v>Lennox Gardens</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>2524231</v>
       </c>
@@ -6000,8 +6306,12 @@
       <c r="U77">
         <v>149.09515265611111</v>
       </c>
-    </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V77" t="str">
+        <f t="shared" si="1"/>
+        <v>Weston Park</v>
+      </c>
+    </row>
+    <row r="78" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>2524232</v>
       </c>
@@ -6065,8 +6375,12 @@
       <c r="U78">
         <v>149.0933929052778</v>
       </c>
-    </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V78" t="str">
+        <f t="shared" si="1"/>
+        <v>Weston Park</v>
+      </c>
+    </row>
+    <row r="79" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>2524233</v>
       </c>
@@ -6128,8 +6442,12 @@
       <c r="U79">
         <v>149.09018163888891</v>
       </c>
-    </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V79" t="str">
+        <f t="shared" si="1"/>
+        <v>Weston Park</v>
+      </c>
+    </row>
+    <row r="80" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>2524234</v>
       </c>
@@ -6193,8 +6511,12 @@
       <c r="U80">
         <v>149.09319869666669</v>
       </c>
-    </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V80" t="str">
+        <f t="shared" si="1"/>
+        <v>Weston Park</v>
+      </c>
+    </row>
+    <row r="81" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>2524235</v>
       </c>
@@ -6256,8 +6578,12 @@
       <c r="U81">
         <v>149.09117874333333</v>
       </c>
-    </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V81" t="str">
+        <f t="shared" si="1"/>
+        <v>Weston Park</v>
+      </c>
+    </row>
+    <row r="82" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>2524236</v>
       </c>
@@ -6319,8 +6645,12 @@
       <c r="U82">
         <v>149.09215420194445</v>
       </c>
-    </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V82" t="str">
+        <f t="shared" si="1"/>
+        <v>Weston Park</v>
+      </c>
+    </row>
+    <row r="83" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>2524237</v>
       </c>
@@ -6376,8 +6706,12 @@
       <c r="U83">
         <v>149.09547073361111</v>
       </c>
-    </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V83" t="str">
+        <f t="shared" si="1"/>
+        <v>Weston Park</v>
+      </c>
+    </row>
+    <row r="84" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>2524239</v>
       </c>
@@ -6439,8 +6773,12 @@
       <c r="U84">
         <v>149.1240221638889</v>
       </c>
-    </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V84" t="str">
+        <f t="shared" si="1"/>
+        <v>Ellenborough Street - Pedestrian Parkland</v>
+      </c>
+    </row>
+    <row r="85" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>2524240</v>
       </c>
@@ -6502,8 +6840,12 @@
       <c r="U85">
         <v>149.07424507444443</v>
       </c>
-    </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V85" t="str">
+        <f t="shared" si="1"/>
+        <v>John Knight Memorial Park</v>
+      </c>
+    </row>
+    <row r="86" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>2524241</v>
       </c>
@@ -6565,8 +6907,12 @@
       <c r="U86">
         <v>149.07420547277778</v>
       </c>
-    </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V86" t="str">
+        <f t="shared" si="1"/>
+        <v>John Knight Memorial Park</v>
+      </c>
+    </row>
+    <row r="87" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>2524243</v>
       </c>
@@ -6622,8 +6968,12 @@
       <c r="U87">
         <v>149.06310779472224</v>
       </c>
-    </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V87" t="str">
+        <f t="shared" si="1"/>
+        <v>Victoria Street Road Verge</v>
+      </c>
+    </row>
+    <row r="88" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>2524245</v>
       </c>
@@ -6687,8 +7037,12 @@
       <c r="U88">
         <v>149.12023597500001</v>
       </c>
-    </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V88" t="str">
+        <f t="shared" si="1"/>
+        <v>Fadden Pines District Park</v>
+      </c>
+    </row>
+    <row r="89" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>2524246</v>
       </c>
@@ -6750,8 +7104,12 @@
       <c r="U89">
         <v>149.12002953916667</v>
       </c>
-    </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V89" t="str">
+        <f t="shared" si="1"/>
+        <v>Fadden Pines District Park</v>
+      </c>
+    </row>
+    <row r="90" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>2524247</v>
       </c>
@@ -6813,8 +7171,12 @@
       <c r="U90">
         <v>149.11936413777778</v>
       </c>
-    </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V90" t="str">
+        <f t="shared" si="1"/>
+        <v>Fadden Pines District Park</v>
+      </c>
+    </row>
+    <row r="91" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>2524249</v>
       </c>
@@ -6878,8 +7240,12 @@
       <c r="U91">
         <v>149.12108924694445</v>
       </c>
-    </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V91" t="str">
+        <f t="shared" si="1"/>
+        <v>Fadden Pines District Park</v>
+      </c>
+    </row>
+    <row r="92" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>2524250</v>
       </c>
@@ -6931,8 +7297,12 @@
       <c r="U92">
         <v>149.11000377166667</v>
       </c>
-    </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V92" t="str">
+        <f t="shared" si="1"/>
+        <v>Candlebark Close Neighbourhood Park</v>
+      </c>
+    </row>
+    <row r="93" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>2524251</v>
       </c>
@@ -6984,8 +7354,12 @@
       <c r="U93">
         <v>149.11013786472222</v>
       </c>
-    </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V93" t="str">
+        <f t="shared" si="1"/>
+        <v>Candlebark Close Neighbourhood Park</v>
+      </c>
+    </row>
+    <row r="94" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>2524252</v>
       </c>
@@ -7041,8 +7415,12 @@
       <c r="U94">
         <v>149.06509157277779</v>
       </c>
-    </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V94" t="str">
+        <f t="shared" si="1"/>
+        <v>Tuggeranong Town Park</v>
+      </c>
+    </row>
+    <row r="95" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>2524253</v>
       </c>
@@ -7094,8 +7472,12 @@
       <c r="U95">
         <v>149.06979267555556</v>
       </c>
-    </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V95" t="str">
+        <f t="shared" si="1"/>
+        <v>Lake Tuggeranong District Park</v>
+      </c>
+    </row>
+    <row r="96" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>2524254</v>
       </c>
@@ -7147,8 +7529,12 @@
       <c r="U96">
         <v>149.07056991083334</v>
       </c>
-    </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V96" t="str">
+        <f t="shared" si="1"/>
+        <v>Lake Tuggeranong District Park</v>
+      </c>
+    </row>
+    <row r="97" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>2524255</v>
       </c>
@@ -7200,8 +7586,12 @@
       <c r="U97">
         <v>149.07150682111111</v>
       </c>
-    </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V97" t="str">
+        <f t="shared" si="1"/>
+        <v>Lake Tuggeranong District Park</v>
+      </c>
+    </row>
+    <row r="98" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>5706719</v>
       </c>
@@ -7247,8 +7637,12 @@
       <c r="Q98" s="2"/>
       <c r="R98" s="2"/>
       <c r="S98" s="2"/>
-    </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V98" t="str">
+        <f t="shared" si="1"/>
+        <v>Bunya Close Pedestrian Parkland</v>
+      </c>
+    </row>
+    <row r="99" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>5823001</v>
       </c>
@@ -7302,8 +7696,12 @@
       <c r="U99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V99" t="str">
+        <f t="shared" si="1"/>
+        <v>Bowen Park</v>
+      </c>
+    </row>
+    <row r="100" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>5823003</v>
       </c>
@@ -7361,8 +7759,12 @@
       <c r="U100">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V100" t="str">
+        <f t="shared" si="1"/>
+        <v>Molonglo Reach Water Ski</v>
+      </c>
+    </row>
+    <row r="101" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>5823004</v>
       </c>
@@ -7420,8 +7822,12 @@
       <c r="U101">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V101" t="str">
+        <f t="shared" si="1"/>
+        <v>Molonglo Reach Water Ski</v>
+      </c>
+    </row>
+    <row r="102" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>6050715</v>
       </c>
@@ -7468,6 +7874,10 @@
       </c>
       <c r="U102">
         <v>0</v>
+      </c>
+      <c r="V102" t="str">
+        <f t="shared" si="1"/>
+        <v>James Harrison Street Neighbourhood Park</v>
       </c>
     </row>
   </sheetData>
@@ -7482,7 +7892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A97" sqref="A2:A97"/>
     </sheetView>
   </sheetViews>

</xml_diff>